<commit_message>
fix and reformant the convert to excel part.
</commit_message>
<xml_diff>
--- a/outputs/test.xlsx
+++ b/outputs/test.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehsan\Desktop\project new step by step\outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\project new step by step\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D4D299-46A0-4950-919B-24C23D0040D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3750791-E379-4782-ADA0-F3FC79197B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cheating Detection Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -43,53 +43,86 @@
     <t>1</t>
   </si>
   <si>
-    <t>100.00</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
-    <t>99.00</t>
-  </si>
-  <si>
-    <t>Undetermined</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>84.00</t>
-  </si>
-  <si>
-    <t>12</t>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
   <si>
     <t>Detailed Cheating Report</t>
   </si>
   <si>
-    <t>Possible cheating between s_1.py and s_10.py with a similarity score of 0.99</t>
-  </si>
-  <si>
-    <t>Possible cheating between s_1.py and s_2.py with a similarity score of 1.00</t>
-  </si>
-  <si>
-    <t>Possible cheating between s_10.py and s_2.py with a similarity score of 0.99</t>
-  </si>
-  <si>
-    <t>Possible cheating between s_11.py and s_12.py with a similarity score of 0.84</t>
+    <t>Possible cheating between s_1.py and s_10.py with an overall score of 0.99 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_1.py and s_2.py with an overall score of 1.00 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_1.py and s_4.py with an overall score of 0.78 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_1.py and s_6.py with an overall score of 0.74 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_1.py and s_8.py with an overall score of 0.75 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_10.py and s_2.py with an overall score of 0.99 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_10.py and s_4.py with an overall score of 0.78 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_10.py and s_6.py with an overall score of 0.74 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_10.py and s_8.py with an overall score of 0.75 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_13.py and s_14.py with an overall score of 0.71 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_2.py and s_4.py with an overall score of 0.78 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_2.py and s_6.py with an overall score of 0.74 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_2.py and s_8.py with an overall score of 0.75 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_4.py and s_6.py with an overall score of 0.73 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_4.py and s_8.py with an overall score of 0.77 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>Possible cheating between s_6.py and s_8.py with an overall score of 0.70 and ML prediction: 1</t>
+  </si>
+  <si>
+    <t>End of Detailed Cheating Report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,17 +132,27 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,15 +161,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF4F81BD"/>
+        <bgColor rgb="FF4F81BD"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor rgb="FFDCE6F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C8E1"/>
+        <bgColor rgb="FFA4C8E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0530BB"/>
+        <bgColor rgb="FF0530BB"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -134,19 +192,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,22 +566,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="79" customWidth="1"/>
-    <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="1" max="1" width="80" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,108 +597,296 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
+        <v>99</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>78</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>74</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>77</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
+        <v>71</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
+        <v>71</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A8:E8"/>
+  <mergeCells count="18">
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>